<commit_message>
calibrated to match MAP estimates
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_malaria.xlsx
+++ b/resources/ResourceFile_malaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="incidence" sheetId="1" r:id="rId1"/>
@@ -363,13 +363,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -475,6 +479,102 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
+        <v>1.8837008808430252E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.22604410570116301</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C17" si="1">B10/12</f>
+        <v>1.8837008808430252E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.22604410570116301</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>1.8837008808430252E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.22604410570116301</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>1.8837008808430252E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.22604410570116301</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>1.8837008808430252E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.22604410570116301</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>1.8837008808430252E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.22604410570116301</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>1.8837008808430252E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.22604410570116301</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>1.8837008808430252E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.22604410570116301</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
         <v>1.8837008808430252E-2</v>
       </c>
     </row>
@@ -487,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
plots showing ITN projections added
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_malaria.xlsx
+++ b/resources/ResourceFile_malaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="45" windowWidth="14835" windowHeight="9360" firstSheet="4" activeTab="5"/>
+    <workbookView minimized="1" xWindow="8115" yWindow="45" windowWidth="14835" windowHeight="9360" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="incidence" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="163">
   <si>
     <t>year</t>
   </si>
@@ -534,6 +534,15 @@
   </si>
   <si>
     <t>p_sev_anaemia_preg</t>
+  </si>
+  <si>
+    <t>MIS_IPTp_1dose</t>
+  </si>
+  <si>
+    <t>MIS_IPTp_3dose</t>
+  </si>
+  <si>
+    <t>MIS_IPTp_2dose</t>
   </si>
 </sst>
 </file>
@@ -1681,7 +1690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1807,15 +1816,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1831,8 +1840,17 @@
       <c r="E1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2000</v>
       </c>
@@ -1846,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -1860,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -1874,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2003</v>
       </c>
@@ -1892,7 +1910,7 @@
         <v>2.0219999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -1910,7 +1928,7 @@
         <v>6.8940000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -1928,7 +1946,7 @@
         <v>0.15816</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -1946,7 +1964,7 @@
         <v>0.14429999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2007</v>
       </c>
@@ -1964,7 +1982,7 @@
         <v>0.17189999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2008</v>
       </c>
@@ -1982,7 +2000,7 @@
         <v>0.19109999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2009</v>
       </c>
@@ -2000,7 +2018,7 @@
         <v>0.17448</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -2018,7 +2036,7 @@
         <v>0.17765999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -2036,7 +2054,7 @@
         <v>0.22319999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -2052,8 +2070,17 @@
       <c r="E14">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>77</v>
+      </c>
+      <c r="G14">
+        <v>54</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -2070,7 +2097,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2014</v>
       </c>
@@ -2086,8 +2113,17 @@
       <c r="E16">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>90</v>
+      </c>
+      <c r="G16">
+        <v>64</v>
+      </c>
+      <c r="H16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -2104,7 +2140,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -2121,7 +2157,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2017</v>
       </c>
@@ -2137,8 +2173,17 @@
       <c r="E19">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>92</v>
+      </c>
+      <c r="G19">
+        <v>76</v>
+      </c>
+      <c r="H19">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2018</v>
       </c>
@@ -2155,7 +2200,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -2172,7 +2217,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2020</v>
       </c>
@@ -2189,7 +2234,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2021</v>
       </c>
@@ -2206,7 +2251,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2022</v>
       </c>
@@ -2223,7 +2268,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2023</v>
       </c>
@@ -2240,7 +2285,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2024</v>
       </c>
@@ -2257,7 +2302,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2025</v>
       </c>
@@ -3767,7 +3812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -3866,7 +3911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView topLeftCell="A215" zoomScale="91" zoomScaleNormal="91" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C253" sqref="C226:C253"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
calibrate malaria cfr to match WHO mortality rates
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_malaria.xlsx
+++ b/resources/ResourceFile_malaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="8115" yWindow="45" windowWidth="14835" windowHeight="9360" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="8115" yWindow="45" windowWidth="14835" windowHeight="9360" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="incidence" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="164">
   <si>
     <t>year</t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>MIS_IPTp_2dose</t>
+  </si>
+  <si>
+    <t>mortality_adjust</t>
   </si>
 </sst>
 </file>
@@ -3810,10 +3813,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3901,6 +3904,14 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3911,7 +3922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView topLeftCell="A212" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="C253" sqref="C226:C253"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove malaria treatment effect to match WHO mortality rates
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_malaria.xlsx
+++ b/resources/ResourceFile_malaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="45" windowWidth="14835" windowHeight="9360" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="8115" yWindow="45" windowWidth="14835" windowHeight="9360" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="incidence" sheetId="1" r:id="rId1"/>
@@ -1191,7 +1191,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E9"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3081,10 +3081,18 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3816,7 +3824,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3893,7 +3901,7 @@
         <v>120</v>
       </c>
       <c r="B9">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reset malaria plots for single runs
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_malaria.xlsx
+++ b/resources/ResourceFile_malaria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="45" windowWidth="14835" windowHeight="9360" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="8115" yWindow="45" windowWidth="14835" windowHeight="9360" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="incidence" sheetId="1" r:id="rId1"/>
@@ -2329,10 +2329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+      <selection activeCell="A20" sqref="A20:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,41 +2603,6 @@
         <v>320.7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2024</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2645,10 +2610,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A20" sqref="A20:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3036,41 +3001,6 @@
         <v>0.26780005666878698</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2024</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3081,7 +3011,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3475,45 +3405,31 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>2018</v>
-      </c>
+      <c r="A20" s="2"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>2019</v>
-      </c>
+      <c r="A21" s="2"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>2020</v>
-      </c>
+      <c r="A22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>2021</v>
-      </c>
+      <c r="A23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>2022</v>
-      </c>
+      <c r="A24" s="2"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>2023</v>
-      </c>
+      <c r="A25" s="2"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>2024</v>
-      </c>
+      <c r="A26" s="2"/>
       <c r="C26" s="2"/>
     </row>
   </sheetData>
@@ -3523,10 +3439,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3767,51 +3683,6 @@
       </c>
       <c r="D17">
         <v>0.42159999999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2024</v>
       </c>
     </row>
   </sheetData>
@@ -3823,7 +3694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>